<commit_message>
overwrite figures with past ones with right size
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/belief_all_mean.xlsx
+++ b/xlsx/country_comparison/belief_all_mean.xlsx
@@ -404,7 +404,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>51.7468895062931</v>
+        <v>51.7468893271431</v>
       </c>
       <c r="C2" t="n">
         <v>58.7165906294257</v>
@@ -427,7 +427,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>54.2040004729188</v>
+        <v>54.2040008566919</v>
       </c>
       <c r="C3" t="n">
         <v>75.7320866764204</v>
@@ -450,7 +450,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>55.1540881609545</v>
+        <v>55.1540879537179</v>
       </c>
       <c r="C4" t="n">
         <v>57.8956679241541</v>
@@ -473,7 +473,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>55.7518322332082</v>
+        <v>55.8431322893747</v>
       </c>
       <c r="C5" t="n">
         <v>72.6238536290562</v>

</xml_diff>